<commit_message>
Update on accuracy graphs on excel files ExperimentComplexityResultsGraph_participants.xlsx and paper. Relocation of results figure to main.tex for controlling the layout.
</commit_message>
<xml_diff>
--- a/Excel/ComplexityAnalysis.xlsx
+++ b/Excel/ComplexityAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b6567a7514cabb0/FABIAN DATA/Kyushu 2021/Research/Paper2Complexity/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2F14C67-F643-46D4-9F11-732B4FBB3B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B2F14C67-F643-46D4-9F11-732B4FBB3B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D5331BB-7883-420F-80EA-E88529B27C0F}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="3225" windowWidth="28800" windowHeight="11055" xr2:uid="{064985ED-ED61-4F28-BAB5-C16312C10D91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{064985ED-ED61-4F28-BAB5-C16312C10D91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -196,6 +192,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,9 +1027,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1068,7 +1067,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1174,7 +1173,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1316,7 +1315,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1324,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7444F8E-B3BE-45BA-90E8-3D70979AE0B4}">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,6 +1403,11 @@
         <v>2.98057498057498E-2</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>